<commit_message>
change gorm version and add area model
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Table</t>
   </si>
@@ -59,10 +59,13 @@
     <t>Field Name</t>
   </si>
   <si>
-    <t>area_ref</t>
-  </si>
-  <si>
-    <t>area_field1</t>
+    <t>laa_AreaRef</t>
+  </si>
+  <si>
+    <t>laa_AreaType</t>
+  </si>
+  <si>
+    <t>laa_areaObjectives</t>
   </si>
   <si>
     <t>obj_ref</t>
@@ -84,6 +87,23 @@
   </si>
   <si>
     <t>tst_ref</t>
+  </si>
+  <si>
+    <t>area_AreaType</t>
+  </si>
+  <si>
+    <t>'type User struct {
+  ID uint             // column name will be `id`
+  Name string         // column name will be `name`
+  Birthday time.Time  // column name will be `birthday`
+  CreatedAt time.Time // column name will be `created_at`
+}
+// Overriding Column Name
+type Animal struct {
+    AnimalId    int64     `gorm:"column:beast_id"`         // set column name to `beast_id`
+    Birthday    time.Time `gorm:"column:day_of_the_beast"` // set column name to `day_of_the_beast`
+    Age         int64     `gorm:"column:age_of_the_beast"` // set column name to `age_of_the_beast`
+}</t>
   </si>
 </sst>
 </file>
@@ -175,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,6 +206,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -265,25 +293,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4210526315789"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.0242914979757"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.7125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.1417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.0242914979757"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.7125506072874"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,23 +322,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -341,8 +370,11 @@
       <c r="J2" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -352,40 +384,43 @@
       <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="G3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="I3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -395,7 +430,7 @@
       <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -415,6 +450,20 @@
       </c>
       <c r="J5" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add objective risk control test models
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Table</t>
   </si>
@@ -35,6 +35,9 @@
     <t>Test</t>
   </si>
   <si>
+    <t>End</t>
+  </si>
+  <si>
     <t>Import</t>
   </si>
   <si>
@@ -68,50 +71,49 @@
     <t>laa_areaObjectives</t>
   </si>
   <si>
-    <t>obj_ref</t>
-  </si>
-  <si>
-    <t>obj_field1</t>
-  </si>
-  <si>
-    <t>rsk_ref</t>
-  </si>
-  <si>
-    <t>rsk_field1</t>
-  </si>
-  <si>
-    <t>ctr_ref</t>
-  </si>
-  <si>
-    <t>ctr_field1</t>
-  </si>
-  <si>
-    <t>tst_ref</t>
+    <t>lro_Title</t>
+  </si>
+  <si>
+    <t>lro_Coverage</t>
+  </si>
+  <si>
+    <t>lrk_RiskRef</t>
+  </si>
+  <si>
+    <t>lrk_Category</t>
+  </si>
+  <si>
+    <t>lct_ControlRef</t>
+  </si>
+  <si>
+    <t>lct_ControlDescription</t>
+  </si>
+  <si>
+    <t>lts_TestRef</t>
+  </si>
+  <si>
+    <t>lts_TestTitle</t>
   </si>
   <si>
     <t>area_AreaType</t>
   </si>
   <si>
-    <t>'type User struct {
-  ID uint             // column name will be `id`
-  Name string         // column name will be `name`
-  Birthday time.Time  // column name will be `birthday`
-  CreatedAt time.Time // column name will be `created_at`
-}
-// Overriding Column Name
-type Animal struct {
-    AnimalId    int64     `gorm:"column:beast_id"`         // set column name to `beast_id`
-    Birthday    time.Time `gorm:"column:day_of_the_beast"` // set column name to `day_of_the_beast`
-    Age         int64     `gorm:"column:age_of_the_beast"` // set column name to `age_of_the_beast`
-}</t>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>lrk_Category1</t>
+  </si>
+  <si>
+    <t>08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -212,8 +214,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -293,10 +295,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -306,12 +308,13 @@
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5748987854251"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.4210526315789"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.7975708502024"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.1417004048583"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.0242914979757"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.7125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.1943319838057"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="55.7894736842105"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.1943319838057"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -338,132 +341,168 @@
       <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>1.1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>11111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>